<commit_message>
feat: custom order support beta
</commit_message>
<xml_diff>
--- a/tests/test_import_headers_experiment/data/import_headers_experiment/100Hz PGA header template.xlsx
+++ b/tests/test_import_headers_experiment/data/import_headers_experiment/100Hz PGA header template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OWN\GitRepos\halt9k\japan-earthquake-data-importer\data\import_headers_experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OWN\GitRepos\halt9k\japan-earthquake-data-importer\tests\test_import_headers_experiment\data\import_headers_experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="24420" windowHeight="11205"/>
+    <workbookView xWindow="1875" yWindow="0" windowWidth="24420" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -1035,27 +1035,37 @@
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>